<commit_message>
Test package fix CM for CLI
Header required for RML_Modules
</commit_message>
<xml_diff>
--- a/mappings/cn_minimal/transformation/conceptual_mappings.xlsx
+++ b/mappings/cn_minimal/transformation/conceptual_mappings.xlsx
@@ -17,14 +17,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataChecksum="RRUe+gY3ALAH5juR4UBCUKv86PwTAuLZN/N98hClkBc="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataChecksum="kFRtKIPm7bYBWLogY224MXFtYEwyDfDYoEZa8lRvBQU="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5453" uniqueCount="2338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5455" uniqueCount="2339">
   <si>
     <t>Field</t>
   </si>
@@ -6801,6 +6801,12 @@
     <t>Change requested by OP</t>
   </si>
   <si>
+    <t>File name</t>
+  </si>
+  <si>
+    <t>Comment (optional)</t>
+  </si>
+  <si>
     <t>technical_mapping_cn_v1.9.rml.ttl</t>
   </si>
   <si>
@@ -7084,9 +7090,6 @@
   </si>
   <si>
     <t>epo:VehicleInformation</t>
-  </si>
-  <si>
-    <t>File name</t>
   </si>
   <si>
     <t>country.json</t>
@@ -7123,7 +7126,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="10.0"/>
       <color theme="1"/>
@@ -7273,6 +7276,11 @@
     <font>
       <u/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -7434,7 +7442,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7679,16 +7687,19 @@
     <xf borderId="0" fillId="10" fontId="11" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="11" fontId="11" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="7" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -31408,8 +31419,16 @@
       <c r="A1" s="92" t="s">
         <v>2232</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="92" t="s">
         <v>2233</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="93" t="s">
+        <v>2234</v>
+      </c>
+      <c r="B2" s="94" t="s">
+        <v>2235</v>
       </c>
     </row>
   </sheetData>
@@ -31435,17 +31454,17 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="95" t="s">
         <v>2179</v>
       </c>
-      <c r="C1" s="95" t="s">
-        <v>2234</v>
-      </c>
-      <c r="D1" s="95" t="s">
-        <v>2235</v>
+      <c r="C1" s="96" t="s">
+        <v>2236</v>
+      </c>
+      <c r="D1" s="96" t="s">
+        <v>2237</v>
       </c>
       <c r="E1" s="76"/>
       <c r="F1" s="18"/>
@@ -31471,2327 +31490,2327 @@
       <c r="Z1" s="18"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="97" t="s">
         <v>1700</v>
       </c>
-      <c r="B2" s="96" t="s">
-        <v>2236</v>
+      <c r="B2" s="97" t="s">
+        <v>2238</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1696</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="97" t="s">
         <v>2182</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>2183</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>328</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="97" t="s">
         <v>472</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="97" t="s">
         <v>2183</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>328</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="97" t="s">
         <v>2170</v>
       </c>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="97" t="s">
         <v>2184</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>487</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="97" t="s">
         <v>997</v>
       </c>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="97" t="s">
         <v>2184</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>995</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="96" t="s">
+      <c r="A7" s="97" t="s">
         <v>685</v>
       </c>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="97" t="s">
         <v>2184</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>681</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="97" t="s">
         <v>1743</v>
       </c>
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="97" t="s">
         <v>2184</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1748</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="96" t="s">
+      <c r="A9" s="97" t="s">
         <v>2150</v>
       </c>
-      <c r="B9" s="96" t="s">
+      <c r="B9" s="97" t="s">
         <v>2184</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>359</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="96" t="s">
+      <c r="A10" s="97" t="s">
         <v>1865</v>
       </c>
-      <c r="B10" s="96" t="s">
-        <v>2238</v>
+      <c r="B10" s="97" t="s">
+        <v>2240</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>834</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="96" t="s">
+      <c r="A11" s="97" t="s">
         <v>583</v>
       </c>
-      <c r="B11" s="96" t="s">
+      <c r="B11" s="97" t="s">
         <v>2203</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>209</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="96" t="s">
-        <v>2239</v>
-      </c>
-      <c r="B12" s="96" t="s">
+      <c r="A12" s="97" t="s">
+        <v>2241</v>
+      </c>
+      <c r="B12" s="97" t="s">
         <v>2203</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1099</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="96" t="s">
-        <v>2240</v>
-      </c>
-      <c r="B13" s="96" t="s">
+      <c r="A13" s="97" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B13" s="97" t="s">
         <v>2203</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>1650</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="97" t="s">
         <v>1349</v>
       </c>
-      <c r="B14" s="96" t="s">
+      <c r="B14" s="97" t="s">
         <v>1351</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>1350</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="96" t="s">
-        <v>2241</v>
-      </c>
-      <c r="B15" s="96" t="s">
+      <c r="A15" s="97" t="s">
+        <v>2243</v>
+      </c>
+      <c r="B15" s="97" t="s">
         <v>1351</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>1350</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="96" t="s">
+      <c r="A16" s="97" t="s">
         <v>1358</v>
       </c>
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="97" t="s">
         <v>1351</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>1350</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="96" t="s">
+      <c r="A17" s="97" t="s">
         <v>1996</v>
       </c>
-      <c r="B17" s="96" t="s">
+      <c r="B17" s="97" t="s">
         <v>1351</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>1994</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="96" t="s">
+      <c r="A18" s="97" t="s">
         <v>1431</v>
       </c>
-      <c r="B18" s="96" t="s">
-        <v>2242</v>
+      <c r="B18" s="97" t="s">
+        <v>2244</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>1350</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E18" s="3"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="96" t="s">
+      <c r="A19" s="97" t="s">
         <v>2059</v>
       </c>
-      <c r="B19" s="96" t="s">
-        <v>2242</v>
+      <c r="B19" s="97" t="s">
+        <v>2244</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>1994</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E19" s="3"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="96" t="s">
+      <c r="A20" s="97" t="s">
         <v>2185</v>
       </c>
-      <c r="B20" s="96" t="s">
+      <c r="B20" s="97" t="s">
         <v>2186</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>328</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E20" s="3"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="96" t="s">
+      <c r="A21" s="97" t="s">
         <v>464</v>
       </c>
-      <c r="B21" s="96" t="s">
+      <c r="B21" s="97" t="s">
         <v>2186</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>328</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E21" s="3"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="96" t="s">
+      <c r="A22" s="97" t="s">
         <v>155</v>
       </c>
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="97" t="s">
         <v>157</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>156</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E22" s="3"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="96" t="s">
-        <v>2243</v>
-      </c>
-      <c r="B23" s="96" t="s">
+      <c r="A23" s="97" t="s">
+        <v>2245</v>
+      </c>
+      <c r="B23" s="97" t="s">
         <v>157</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>163</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E23" s="3"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="96" t="s">
+      <c r="A24" s="97" t="s">
         <v>2073</v>
       </c>
-      <c r="B24" s="96" t="s">
-        <v>2244</v>
+      <c r="B24" s="97" t="s">
+        <v>2246</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>2091</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E24" s="3"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="96" t="s">
+      <c r="A25" s="97" t="s">
         <v>2139</v>
       </c>
-      <c r="B25" s="96" t="s">
+      <c r="B25" s="97" t="s">
         <v>2187</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>331</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E25" s="3"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="96" t="s">
+      <c r="A26" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="96" t="s">
-        <v>2245</v>
+      <c r="B26" s="97" t="s">
+        <v>2247</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E26" s="3"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="96" t="s">
+      <c r="A27" s="97" t="s">
         <v>1409</v>
       </c>
-      <c r="B27" s="96" t="s">
-        <v>2246</v>
+      <c r="B27" s="97" t="s">
+        <v>2248</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>1406</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E27" s="3"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="96" t="s">
+      <c r="A28" s="97" t="s">
         <v>2041</v>
       </c>
-      <c r="B28" s="96" t="s">
-        <v>2246</v>
+      <c r="B28" s="97" t="s">
+        <v>2248</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>2029</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E28" s="3"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="96" t="s">
+      <c r="A29" s="97" t="s">
         <v>1298</v>
       </c>
-      <c r="B29" s="96" t="s">
-        <v>2246</v>
+      <c r="B29" s="97" t="s">
+        <v>2248</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>1314</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E29" s="3"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="96" t="s">
+      <c r="A30" s="97" t="s">
         <v>2137</v>
       </c>
-      <c r="B30" s="96" t="s">
+      <c r="B30" s="97" t="s">
         <v>2188</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>331</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E30" s="3"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="96" t="s">
+      <c r="A31" s="97" t="s">
         <v>624</v>
       </c>
-      <c r="B31" s="96" t="s">
+      <c r="B31" s="97" t="s">
         <v>678</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>244</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E31" s="3"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="96" t="s">
+      <c r="A32" s="97" t="s">
         <v>866</v>
       </c>
-      <c r="B32" s="96" t="s">
+      <c r="B32" s="97" t="s">
         <v>678</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>1529</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E32" s="3"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="96" t="s">
+      <c r="A33" s="97" t="s">
         <v>267</v>
       </c>
-      <c r="B33" s="96" t="s">
+      <c r="B33" s="97" t="s">
         <v>678</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>681</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E33" s="3"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="96" t="s">
+      <c r="A34" s="97" t="s">
         <v>627</v>
       </c>
-      <c r="B34" s="96" t="s">
+      <c r="B34" s="97" t="s">
         <v>678</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>272</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E34" s="3"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="96" t="s">
+      <c r="A35" s="97" t="s">
         <v>1115</v>
       </c>
-      <c r="B35" s="96" t="s">
-        <v>2247</v>
+      <c r="B35" s="97" t="s">
+        <v>2249</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>1149</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E35" s="3"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="96" t="s">
+      <c r="A36" s="97" t="s">
         <v>1075</v>
       </c>
-      <c r="B36" s="96" t="s">
-        <v>2248</v>
+      <c r="B36" s="97" t="s">
+        <v>2250</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>1069</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E36" s="3"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="96" t="s">
-        <v>2249</v>
-      </c>
-      <c r="B37" s="96" t="s">
-        <v>2250</v>
+      <c r="A37" s="97" t="s">
+        <v>2251</v>
+      </c>
+      <c r="B37" s="97" t="s">
+        <v>2252</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>1230</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E37" s="3"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="96" t="s">
-        <v>2251</v>
-      </c>
-      <c r="B38" s="96" t="s">
-        <v>2252</v>
+      <c r="A38" s="97" t="s">
+        <v>2253</v>
+      </c>
+      <c r="B38" s="97" t="s">
+        <v>2254</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>1214</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E38" s="3"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="96" t="s">
+      <c r="A39" s="97" t="s">
         <v>745</v>
       </c>
-      <c r="B39" s="96" t="s">
+      <c r="B39" s="97" t="s">
         <v>740</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>739</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E39" s="3"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="96" t="s">
+      <c r="A40" s="97" t="s">
         <v>1108</v>
       </c>
-      <c r="B40" s="96" t="s">
-        <v>2253</v>
+      <c r="B40" s="97" t="s">
+        <v>2255</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>1146</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E40" s="3"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="96" t="s">
+      <c r="A41" s="97" t="s">
         <v>1158</v>
       </c>
-      <c r="B41" s="96" t="s">
-        <v>2254</v>
+      <c r="B41" s="97" t="s">
+        <v>2256</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>1152</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E41" s="3"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="96" t="s">
+      <c r="A42" s="97" t="s">
         <v>1122</v>
       </c>
-      <c r="B42" s="96" t="s">
-        <v>2255</v>
+      <c r="B42" s="97" t="s">
+        <v>2257</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>1123</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E42" s="3"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="96" t="s">
+      <c r="A43" s="97" t="s">
         <v>1588</v>
       </c>
-      <c r="B43" s="96" t="s">
-        <v>2256</v>
+      <c r="B43" s="97" t="s">
+        <v>2258</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>1579</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E43" s="3"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="96" t="s">
+      <c r="A44" s="97" t="s">
         <v>924</v>
       </c>
-      <c r="B44" s="96" t="s">
-        <v>2256</v>
+      <c r="B44" s="97" t="s">
+        <v>2258</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>920</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E44" s="3"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
-      <c r="A45" s="96" t="s">
+      <c r="A45" s="97" t="s">
         <v>2146</v>
       </c>
-      <c r="B45" s="96" t="s">
+      <c r="B45" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>331</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E45" s="3"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="96" t="s">
+      <c r="A46" s="97" t="s">
         <v>1939</v>
       </c>
-      <c r="B46" s="96" t="s">
+      <c r="B46" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>1937</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E46" s="3"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
-      <c r="A47" s="96" t="s">
+      <c r="A47" s="97" t="s">
         <v>2133</v>
       </c>
-      <c r="B47" s="96" t="s">
+      <c r="B47" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>350</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E47" s="3"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
-      <c r="A48" s="96" t="s">
-        <v>2257</v>
-      </c>
-      <c r="B48" s="96" t="s">
+      <c r="A48" s="97" t="s">
+        <v>2259</v>
+      </c>
+      <c r="B48" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>1099</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E48" s="3"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
-      <c r="A49" s="96" t="s">
-        <v>2258</v>
-      </c>
-      <c r="B49" s="96" t="s">
+      <c r="A49" s="97" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B49" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>1650</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E49" s="3"/>
     </row>
     <row r="50" ht="12.75" customHeight="1">
-      <c r="A50" s="96" t="s">
-        <v>2259</v>
-      </c>
-      <c r="B50" s="96" t="s">
+      <c r="A50" s="97" t="s">
+        <v>2261</v>
+      </c>
+      <c r="B50" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>1230</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E50" s="3"/>
     </row>
     <row r="51" ht="12.75" customHeight="1">
-      <c r="A51" s="96" t="s">
-        <v>2260</v>
-      </c>
-      <c r="B51" s="96" t="s">
+      <c r="A51" s="97" t="s">
+        <v>2262</v>
+      </c>
+      <c r="B51" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>1214</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E51" s="3"/>
     </row>
     <row r="52" ht="12.75" customHeight="1">
-      <c r="A52" s="96" t="s">
-        <v>2261</v>
-      </c>
-      <c r="B52" s="96" t="s">
+      <c r="A52" s="97" t="s">
+        <v>2263</v>
+      </c>
+      <c r="B52" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>1889</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E52" s="3"/>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="96" t="s">
-        <v>2262</v>
-      </c>
-      <c r="B53" s="96" t="s">
+      <c r="A53" s="97" t="s">
+        <v>2264</v>
+      </c>
+      <c r="B53" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>1099</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E53" s="3"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
-      <c r="A54" s="96" t="s">
-        <v>2263</v>
-      </c>
-      <c r="B54" s="96" t="s">
+      <c r="A54" s="97" t="s">
+        <v>2265</v>
+      </c>
+      <c r="B54" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>1898</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E54" s="3"/>
     </row>
     <row r="55" ht="12.75" customHeight="1">
-      <c r="A55" s="96" t="s">
-        <v>2264</v>
-      </c>
-      <c r="B55" s="96" t="s">
+      <c r="A55" s="97" t="s">
+        <v>2266</v>
+      </c>
+      <c r="B55" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>1898</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E55" s="3"/>
     </row>
     <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" s="96" t="s">
-        <v>2265</v>
-      </c>
-      <c r="B56" s="96" t="s">
+      <c r="A56" s="97" t="s">
+        <v>2267</v>
+      </c>
+      <c r="B56" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>1099</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E56" s="3"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
-      <c r="A57" s="96" t="s">
-        <v>2266</v>
-      </c>
-      <c r="B57" s="96" t="s">
+      <c r="A57" s="97" t="s">
+        <v>2268</v>
+      </c>
+      <c r="B57" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>1193</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E57" s="3"/>
     </row>
     <row r="58" ht="12.75" customHeight="1">
-      <c r="A58" s="96" t="s">
+      <c r="A58" s="97" t="s">
         <v>1135</v>
       </c>
-      <c r="B58" s="96" t="s">
+      <c r="B58" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>1123</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E58" s="3"/>
     </row>
     <row r="59" ht="12.75" customHeight="1">
-      <c r="A59" s="96" t="s">
+      <c r="A59" s="97" t="s">
         <v>829</v>
       </c>
-      <c r="B59" s="96" t="s">
+      <c r="B59" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>823</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E59" s="3"/>
     </row>
     <row r="60" ht="12.75" customHeight="1">
-      <c r="A60" s="96" t="s">
+      <c r="A60" s="97" t="s">
         <v>815</v>
       </c>
-      <c r="B60" s="96" t="s">
+      <c r="B60" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>809</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E60" s="3"/>
     </row>
     <row r="61" ht="12.75" customHeight="1">
-      <c r="A61" s="96" t="s">
+      <c r="A61" s="97" t="s">
         <v>1931</v>
       </c>
-      <c r="B61" s="96" t="s">
+      <c r="B61" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>1927</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E61" s="3"/>
     </row>
     <row r="62" ht="12.75" customHeight="1">
-      <c r="A62" s="96" t="s">
+      <c r="A62" s="97" t="s">
         <v>803</v>
       </c>
-      <c r="B62" s="96" t="s">
+      <c r="B62" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>797</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E62" s="3"/>
     </row>
     <row r="63" ht="12.75" customHeight="1">
-      <c r="A63" s="96" t="s">
+      <c r="A63" s="97" t="s">
         <v>81</v>
       </c>
-      <c r="B63" s="96" t="s">
+      <c r="B63" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E63" s="3"/>
     </row>
     <row r="64" ht="12.75" customHeight="1">
-      <c r="A64" s="96" t="s">
+      <c r="A64" s="97" t="s">
         <v>2190</v>
       </c>
-      <c r="B64" s="96" t="s">
+      <c r="B64" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>226</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E64" s="3"/>
     </row>
     <row r="65" ht="12.75" customHeight="1">
-      <c r="A65" s="96" t="s">
-        <v>2267</v>
-      </c>
-      <c r="B65" s="96" t="s">
+      <c r="A65" s="97" t="s">
+        <v>2269</v>
+      </c>
+      <c r="B65" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>2065</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E65" s="3"/>
     </row>
     <row r="66" ht="12.75" customHeight="1">
-      <c r="A66" s="96" t="s">
-        <v>2268</v>
-      </c>
-      <c r="B66" s="96" t="s">
+      <c r="A66" s="97" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B66" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>837</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E66" s="3"/>
     </row>
     <row r="67" ht="12.75" customHeight="1">
-      <c r="A67" s="96" t="s">
+      <c r="A67" s="97" t="s">
         <v>844</v>
       </c>
-      <c r="B67" s="96" t="s">
+      <c r="B67" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>837</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E67" s="3"/>
     </row>
     <row r="68" ht="12.75" customHeight="1">
-      <c r="A68" s="96" t="s">
+      <c r="A68" s="97" t="s">
         <v>599</v>
       </c>
-      <c r="B68" s="96" t="s">
+      <c r="B68" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>603</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E68" s="3"/>
     </row>
     <row r="69" ht="12.75" customHeight="1">
-      <c r="A69" s="96" t="s">
+      <c r="A69" s="97" t="s">
         <v>2191</v>
       </c>
-      <c r="B69" s="96" t="s">
+      <c r="B69" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E69" s="3"/>
     </row>
     <row r="70" ht="12.75" customHeight="1">
-      <c r="A70" s="96" t="s">
+      <c r="A70" s="97" t="s">
         <v>1858</v>
       </c>
-      <c r="B70" s="96" t="s">
+      <c r="B70" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>1791</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E70" s="3"/>
     </row>
     <row r="71" ht="12.75" customHeight="1">
-      <c r="A71" s="96" t="s">
+      <c r="A71" s="97" t="s">
         <v>2098</v>
       </c>
-      <c r="B71" s="96" t="s">
+      <c r="B71" s="97" t="s">
         <v>2189</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>2094</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E71" s="3"/>
     </row>
     <row r="72" ht="12.75" customHeight="1">
-      <c r="A72" s="96" t="s">
+      <c r="A72" s="97" t="s">
         <v>950</v>
       </c>
-      <c r="B72" s="96" t="s">
-        <v>2269</v>
+      <c r="B72" s="97" t="s">
+        <v>2271</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>946</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E72" s="3"/>
     </row>
     <row r="73" ht="12.75" customHeight="1">
-      <c r="A73" s="96" t="s">
+      <c r="A73" s="97" t="s">
         <v>2192</v>
       </c>
-      <c r="B73" s="96" t="s">
+      <c r="B73" s="97" t="s">
         <v>2193</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>328</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E73" s="3"/>
     </row>
     <row r="74" ht="12.75" customHeight="1">
-      <c r="A74" s="96" t="s">
+      <c r="A74" s="97" t="s">
         <v>455</v>
       </c>
-      <c r="B74" s="96" t="s">
+      <c r="B74" s="97" t="s">
         <v>2193</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>328</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E74" s="3"/>
     </row>
     <row r="75" ht="12.75" customHeight="1">
-      <c r="A75" s="96" t="s">
+      <c r="A75" s="97" t="s">
         <v>990</v>
       </c>
-      <c r="B75" s="96" t="s">
-        <v>2270</v>
+      <c r="B75" s="97" t="s">
+        <v>2272</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>995</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E75" s="3"/>
     </row>
     <row r="76" ht="12.75" customHeight="1">
-      <c r="A76" s="96" t="s">
+      <c r="A76" s="97" t="s">
         <v>714</v>
       </c>
-      <c r="B76" s="96" t="s">
-        <v>2270</v>
+      <c r="B76" s="97" t="s">
+        <v>2272</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>681</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E76" s="3"/>
     </row>
     <row r="77" ht="12.75" customHeight="1">
-      <c r="A77" s="96" t="s">
+      <c r="A77" s="97" t="s">
         <v>569</v>
       </c>
-      <c r="B77" s="96" t="s">
+      <c r="B77" s="97" t="s">
         <v>824</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>823</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E77" s="3"/>
     </row>
     <row r="78" ht="12.75" customHeight="1">
-      <c r="A78" s="96" t="s">
+      <c r="A78" s="97" t="s">
         <v>1665</v>
       </c>
-      <c r="B78" s="96" t="s">
+      <c r="B78" s="97" t="s">
         <v>824</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>1663</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E78" s="3"/>
     </row>
     <row r="79" ht="12.75" customHeight="1">
-      <c r="A79" s="96" t="s">
-        <v>2271</v>
-      </c>
-      <c r="B79" s="96" t="s">
+      <c r="A79" s="97" t="s">
+        <v>2273</v>
+      </c>
+      <c r="B79" s="97" t="s">
         <v>824</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>1230</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E79" s="3"/>
     </row>
     <row r="80" ht="12.75" customHeight="1">
-      <c r="A80" s="96" t="s">
-        <v>2272</v>
-      </c>
-      <c r="B80" s="96" t="s">
+      <c r="A80" s="97" t="s">
+        <v>2274</v>
+      </c>
+      <c r="B80" s="97" t="s">
         <v>824</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>1214</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E80" s="3"/>
     </row>
     <row r="81" ht="12.75" customHeight="1">
-      <c r="A81" s="96" t="s">
+      <c r="A81" s="97" t="s">
         <v>1921</v>
       </c>
-      <c r="B81" s="96" t="s">
+      <c r="B81" s="97" t="s">
         <v>824</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>1889</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E81" s="3"/>
     </row>
     <row r="82" ht="12.75" customHeight="1">
-      <c r="A82" s="96" t="s">
-        <v>2273</v>
-      </c>
-      <c r="B82" s="96" t="s">
+      <c r="A82" s="97" t="s">
+        <v>2275</v>
+      </c>
+      <c r="B82" s="97" t="s">
         <v>824</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>1193</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E82" s="3"/>
     </row>
     <row r="83" ht="12.75" customHeight="1">
-      <c r="A83" s="96" t="s">
+      <c r="A83" s="97" t="s">
         <v>588</v>
       </c>
-      <c r="B83" s="96" t="s">
+      <c r="B83" s="97" t="s">
         <v>824</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E83" s="3"/>
     </row>
     <row r="84" ht="12.75" customHeight="1">
-      <c r="A84" s="96" t="s">
+      <c r="A84" s="97" t="s">
         <v>1953</v>
       </c>
-      <c r="B84" s="96" t="s">
+      <c r="B84" s="97" t="s">
         <v>824</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>1937</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E84" s="3"/>
     </row>
     <row r="85" ht="12.75" customHeight="1">
-      <c r="A85" s="96" t="s">
+      <c r="A85" s="97" t="s">
         <v>808</v>
       </c>
-      <c r="B85" s="96" t="s">
+      <c r="B85" s="97" t="s">
         <v>824</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>809</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E85" s="3"/>
     </row>
     <row r="86" ht="12.75" customHeight="1">
-      <c r="A86" s="96" t="s">
-        <v>2274</v>
-      </c>
-      <c r="B86" s="96" t="s">
-        <v>2275</v>
+      <c r="A86" s="97" t="s">
+        <v>2276</v>
+      </c>
+      <c r="B86" s="97" t="s">
+        <v>2277</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>1184</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E86" s="3"/>
     </row>
     <row r="87" ht="12.75" customHeight="1">
-      <c r="A87" s="96" t="s">
+      <c r="A87" s="97" t="s">
         <v>1926</v>
       </c>
-      <c r="B87" s="96" t="s">
+      <c r="B87" s="97" t="s">
         <v>1928</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>1937</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E87" s="3"/>
     </row>
     <row r="88" ht="12.75" customHeight="1">
-      <c r="A88" s="96" t="s">
-        <v>2276</v>
-      </c>
-      <c r="B88" s="96" t="s">
-        <v>2277</v>
+      <c r="A88" s="97" t="s">
+        <v>2278</v>
+      </c>
+      <c r="B88" s="97" t="s">
+        <v>2279</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>1927</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E88" s="3"/>
     </row>
     <row r="89" ht="12.75" customHeight="1">
-      <c r="A89" s="96" t="s">
+      <c r="A89" s="97" t="s">
         <v>796</v>
       </c>
-      <c r="B89" s="96" t="s">
+      <c r="B89" s="97" t="s">
         <v>1928</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>797</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E89" s="3"/>
     </row>
     <row r="90" ht="12.75" customHeight="1">
-      <c r="A90" s="96" t="s">
-        <v>2278</v>
-      </c>
-      <c r="B90" s="96" t="s">
-        <v>2279</v>
+      <c r="A90" s="97" t="s">
+        <v>2280</v>
+      </c>
+      <c r="B90" s="97" t="s">
+        <v>2281</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>1966</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E90" s="3"/>
     </row>
     <row r="91" ht="12.75" customHeight="1">
-      <c r="A91" s="96" t="s">
-        <v>2280</v>
-      </c>
-      <c r="B91" s="96" t="s">
-        <v>2279</v>
+      <c r="A91" s="97" t="s">
+        <v>2282</v>
+      </c>
+      <c r="B91" s="97" t="s">
+        <v>2281</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>1966</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E91" s="3"/>
     </row>
     <row r="92" ht="12.75" customHeight="1">
-      <c r="A92" s="96" t="s">
-        <v>2281</v>
-      </c>
-      <c r="B92" s="96" t="s">
-        <v>2282</v>
+      <c r="A92" s="97" t="s">
+        <v>2283</v>
+      </c>
+      <c r="B92" s="97" t="s">
+        <v>2284</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>1889</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E92" s="3"/>
     </row>
     <row r="93" ht="12.75" customHeight="1">
-      <c r="A93" s="96" t="s">
+      <c r="A93" s="97" t="s">
         <v>899</v>
       </c>
-      <c r="B93" s="96" t="s">
-        <v>2283</v>
+      <c r="B93" s="97" t="s">
+        <v>2285</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>897</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E93" s="3"/>
     </row>
     <row r="94" ht="12.75" customHeight="1">
-      <c r="A94" s="96" t="s">
+      <c r="A94" s="97" t="s">
         <v>1961</v>
       </c>
-      <c r="B94" s="96" t="s">
-        <v>2283</v>
+      <c r="B94" s="97" t="s">
+        <v>2285</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>1959</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E94" s="3"/>
     </row>
     <row r="95" ht="12.75" customHeight="1">
-      <c r="A95" s="96" t="s">
+      <c r="A95" s="97" t="s">
         <v>635</v>
       </c>
-      <c r="B95" s="96" t="s">
-        <v>2283</v>
+      <c r="B95" s="97" t="s">
+        <v>2285</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>631</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E95" s="3"/>
     </row>
     <row r="96" ht="12.75" customHeight="1">
-      <c r="A96" s="96" t="s">
+      <c r="A96" s="97" t="s">
         <v>644</v>
       </c>
-      <c r="B96" s="96" t="s">
-        <v>2283</v>
+      <c r="B96" s="97" t="s">
+        <v>2285</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>640</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E96" s="3"/>
     </row>
     <row r="97" ht="12.75" customHeight="1">
-      <c r="A97" s="96" t="s">
-        <v>2284</v>
-      </c>
-      <c r="B97" s="96" t="s">
-        <v>2283</v>
+      <c r="A97" s="97" t="s">
+        <v>2286</v>
+      </c>
+      <c r="B97" s="97" t="s">
+        <v>2285</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>1184</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E97" s="3"/>
     </row>
     <row r="98" ht="12.75" customHeight="1">
-      <c r="A98" s="96" t="s">
+      <c r="A98" s="97" t="s">
         <v>1982</v>
       </c>
-      <c r="B98" s="96" t="s">
-        <v>2283</v>
+      <c r="B98" s="97" t="s">
+        <v>2285</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>1980</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E98" s="3"/>
     </row>
     <row r="99" ht="12.75" customHeight="1">
-      <c r="A99" s="96" t="s">
+      <c r="A99" s="97" t="s">
         <v>1970</v>
       </c>
-      <c r="B99" s="96" t="s">
-        <v>2283</v>
+      <c r="B99" s="97" t="s">
+        <v>2285</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>1966</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E99" s="3"/>
     </row>
     <row r="100" ht="12.75" customHeight="1">
-      <c r="A100" s="96" t="s">
+      <c r="A100" s="97" t="s">
         <v>1324</v>
       </c>
-      <c r="B100" s="96" t="s">
-        <v>2285</v>
+      <c r="B100" s="97" t="s">
+        <v>2287</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>1347</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E100" s="3"/>
     </row>
     <row r="101" ht="12.75" customHeight="1">
-      <c r="A101" s="96" t="s">
+      <c r="A101" s="97" t="s">
         <v>1599</v>
       </c>
-      <c r="B101" s="96" t="s">
-        <v>2286</v>
+      <c r="B101" s="97" t="s">
+        <v>2288</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>1595</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E101" s="3"/>
     </row>
     <row r="102" ht="12.75" customHeight="1">
-      <c r="A102" s="96" t="s">
+      <c r="A102" s="97" t="s">
         <v>48</v>
       </c>
-      <c r="B102" s="96" t="s">
+      <c r="B102" s="97" t="s">
         <v>50</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>137</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E102" s="3"/>
     </row>
     <row r="103" ht="12.75" customHeight="1">
-      <c r="A103" s="96" t="s">
+      <c r="A103" s="97" t="s">
         <v>2064</v>
       </c>
-      <c r="B103" s="96" t="s">
+      <c r="B103" s="97" t="s">
         <v>50</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>2065</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E103" s="3"/>
     </row>
     <row r="104" ht="12.75" customHeight="1">
-      <c r="A104" s="96" t="s">
+      <c r="A104" s="97" t="s">
         <v>2194</v>
       </c>
-      <c r="B104" s="96" t="s">
+      <c r="B104" s="97" t="s">
         <v>50</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>226</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E104" s="3"/>
     </row>
     <row r="105" ht="12.75" customHeight="1">
-      <c r="A105" s="96" t="s">
-        <v>2287</v>
-      </c>
-      <c r="B105" s="96" t="s">
+      <c r="A105" s="97" t="s">
+        <v>2289</v>
+      </c>
+      <c r="B105" s="97" t="s">
         <v>50</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>2065</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E105" s="3"/>
     </row>
     <row r="106" ht="12.75" customHeight="1">
-      <c r="A106" s="96" t="s">
+      <c r="A106" s="97" t="s">
         <v>1728</v>
       </c>
-      <c r="B106" s="96" t="s">
-        <v>2288</v>
+      <c r="B106" s="97" t="s">
+        <v>2290</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>1724</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E106" s="3"/>
     </row>
     <row r="107" ht="12.75" customHeight="1">
-      <c r="A107" s="96" t="s">
+      <c r="A107" s="97" t="s">
         <v>573</v>
       </c>
-      <c r="B107" s="96" t="s">
+      <c r="B107" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>331</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E107" s="3"/>
     </row>
     <row r="108" ht="12.75" customHeight="1">
-      <c r="A108" s="96" t="s">
+      <c r="A108" s="97" t="s">
         <v>2167</v>
       </c>
-      <c r="B108" s="96" t="s">
+      <c r="B108" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>487</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E108" s="3"/>
     </row>
     <row r="109" ht="12.75" customHeight="1">
-      <c r="A109" s="96" t="s">
+      <c r="A109" s="97" t="s">
         <v>2195</v>
       </c>
-      <c r="B109" s="96" t="s">
+      <c r="B109" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>328</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E109" s="3"/>
     </row>
     <row r="110" ht="12.75" customHeight="1">
-      <c r="A110" s="96" t="s">
+      <c r="A110" s="97" t="s">
         <v>2143</v>
       </c>
-      <c r="B110" s="96" t="s">
+      <c r="B110" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>331</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E110" s="3"/>
     </row>
     <row r="111" ht="12.75" customHeight="1">
-      <c r="A111" s="96" t="s">
-        <v>2289</v>
-      </c>
-      <c r="B111" s="96" t="s">
+      <c r="A111" s="97" t="s">
+        <v>2291</v>
+      </c>
+      <c r="B111" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>1099</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E111" s="3"/>
     </row>
     <row r="112" ht="12.75" customHeight="1">
-      <c r="A112" s="96" t="s">
-        <v>2290</v>
-      </c>
-      <c r="B112" s="96" t="s">
+      <c r="A112" s="97" t="s">
+        <v>2292</v>
+      </c>
+      <c r="B112" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>1650</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E112" s="3"/>
     </row>
     <row r="113" ht="12.75" customHeight="1">
-      <c r="A113" s="96" t="s">
+      <c r="A113" s="97" t="s">
         <v>2196</v>
       </c>
-      <c r="B113" s="96" t="s">
+      <c r="B113" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>328</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E113" s="3"/>
     </row>
     <row r="114" ht="12.75" customHeight="1">
-      <c r="A114" s="96" t="s">
-        <v>2291</v>
-      </c>
-      <c r="B114" s="96" t="s">
+      <c r="A114" s="97" t="s">
+        <v>2293</v>
+      </c>
+      <c r="B114" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>1230</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E114" s="3"/>
     </row>
     <row r="115" ht="12.75" customHeight="1">
-      <c r="A115" s="96" t="s">
-        <v>2292</v>
-      </c>
-      <c r="B115" s="96" t="s">
+      <c r="A115" s="97" t="s">
+        <v>2294</v>
+      </c>
+      <c r="B115" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>1214</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E115" s="3"/>
     </row>
     <row r="116" ht="12.75" customHeight="1">
-      <c r="A116" s="96" t="s">
+      <c r="A116" s="97" t="s">
         <v>2197</v>
       </c>
-      <c r="B116" s="96" t="s">
+      <c r="B116" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>328</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E116" s="3"/>
     </row>
     <row r="117" ht="12.75" customHeight="1">
-      <c r="A117" s="96" t="s">
-        <v>2293</v>
-      </c>
-      <c r="B117" s="96" t="s">
+      <c r="A117" s="97" t="s">
+        <v>2295</v>
+      </c>
+      <c r="B117" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>1889</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E117" s="3"/>
     </row>
     <row r="118" ht="12.75" customHeight="1">
-      <c r="A118" s="96" t="s">
-        <v>2294</v>
-      </c>
-      <c r="B118" s="96" t="s">
+      <c r="A118" s="97" t="s">
+        <v>2296</v>
+      </c>
+      <c r="B118" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>1099</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E118" s="3"/>
     </row>
     <row r="119" ht="12.75" customHeight="1">
-      <c r="A119" s="96" t="s">
-        <v>2295</v>
-      </c>
-      <c r="B119" s="96" t="s">
+      <c r="A119" s="97" t="s">
+        <v>2297</v>
+      </c>
+      <c r="B119" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>1889</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E119" s="3"/>
     </row>
     <row r="120" ht="12.75" customHeight="1">
-      <c r="A120" s="96" t="s">
-        <v>2296</v>
-      </c>
-      <c r="B120" s="96" t="s">
+      <c r="A120" s="97" t="s">
+        <v>2298</v>
+      </c>
+      <c r="B120" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>1898</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E120" s="3"/>
     </row>
     <row r="121" ht="12.75" customHeight="1">
-      <c r="A121" s="96" t="s">
-        <v>2297</v>
-      </c>
-      <c r="B121" s="96" t="s">
+      <c r="A121" s="97" t="s">
+        <v>2299</v>
+      </c>
+      <c r="B121" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>1099</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E121" s="3"/>
     </row>
     <row r="122" ht="12.75" customHeight="1">
-      <c r="A122" s="96" t="s">
-        <v>2298</v>
-      </c>
-      <c r="B122" s="96" t="s">
+      <c r="A122" s="97" t="s">
+        <v>2300</v>
+      </c>
+      <c r="B122" s="97" t="s">
         <v>347</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>1193</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E122" s="3"/>
     </row>
     <row r="123" ht="12.75" customHeight="1">
-      <c r="A123" s="96" t="s">
+      <c r="A123" s="97" t="s">
         <v>1479</v>
       </c>
-      <c r="B123" s="96" t="s">
-        <v>2299</v>
+      <c r="B123" s="97" t="s">
+        <v>2301</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>1475</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E123" s="3"/>
     </row>
     <row r="124" ht="12.75" customHeight="1">
-      <c r="A124" s="96" t="s">
+      <c r="A124" s="97" t="s">
         <v>1026</v>
       </c>
-      <c r="B124" s="96" t="s">
-        <v>2300</v>
+      <c r="B124" s="97" t="s">
+        <v>2302</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>1022</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E124" s="3"/>
     </row>
     <row r="125" ht="12.75" customHeight="1">
-      <c r="A125" s="96" t="s">
-        <v>2301</v>
-      </c>
-      <c r="B125" s="96" t="s">
-        <v>2302</v>
+      <c r="A125" s="97" t="s">
+        <v>2303</v>
+      </c>
+      <c r="B125" s="97" t="s">
+        <v>2304</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>837</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E125" s="3"/>
     </row>
     <row r="126" ht="12.75" customHeight="1">
-      <c r="A126" s="96" t="s">
+      <c r="A126" s="97" t="s">
         <v>836</v>
       </c>
-      <c r="B126" s="96" t="s">
-        <v>2303</v>
+      <c r="B126" s="97" t="s">
+        <v>2305</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>837</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E126" s="3"/>
     </row>
     <row r="127" ht="12.75" customHeight="1">
-      <c r="A127" s="96" t="s">
+      <c r="A127" s="97" t="s">
         <v>243</v>
       </c>
-      <c r="B127" s="96" t="s">
+      <c r="B127" s="97" t="s">
         <v>245</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>308</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E127" s="3"/>
     </row>
     <row r="128" ht="12.75" customHeight="1">
-      <c r="A128" s="96" t="s">
-        <v>2304</v>
-      </c>
-      <c r="B128" s="96" t="s">
+      <c r="A128" s="97" t="s">
+        <v>2306</v>
+      </c>
+      <c r="B128" s="97" t="s">
         <v>245</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>611</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E128" s="3"/>
     </row>
     <row r="129" ht="12.75" customHeight="1">
-      <c r="A129" s="96" t="s">
-        <v>2305</v>
-      </c>
-      <c r="B129" s="96" t="s">
+      <c r="A129" s="97" t="s">
+        <v>2307</v>
+      </c>
+      <c r="B129" s="97" t="s">
         <v>245</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>308</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E129" s="3"/>
     </row>
     <row r="130" ht="12.75" customHeight="1">
-      <c r="A130" s="96" t="s">
-        <v>2306</v>
-      </c>
-      <c r="B130" s="96" t="s">
+      <c r="A130" s="97" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B130" s="97" t="s">
         <v>245</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>308</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E130" s="3"/>
     </row>
     <row r="131" ht="12.75" customHeight="1">
-      <c r="A131" s="96" t="s">
+      <c r="A131" s="97" t="s">
         <v>286</v>
       </c>
-      <c r="B131" s="96" t="s">
+      <c r="B131" s="97" t="s">
         <v>245</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>224</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E131" s="3"/>
     </row>
     <row r="132" ht="12.75" customHeight="1">
-      <c r="A132" s="96" t="s">
+      <c r="A132" s="97" t="s">
         <v>2199</v>
       </c>
-      <c r="B132" s="96" t="s">
+      <c r="B132" s="97" t="s">
         <v>245</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E132" s="3"/>
     </row>
     <row r="133" ht="12.75" customHeight="1">
-      <c r="A133" s="96" t="s">
+      <c r="A133" s="97" t="s">
         <v>303</v>
       </c>
-      <c r="B133" s="96" t="s">
+      <c r="B133" s="97" t="s">
         <v>2200</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>224</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E133" s="3"/>
     </row>
     <row r="134" ht="12.75" customHeight="1">
-      <c r="A134" s="96" t="s">
+      <c r="A134" s="97" t="s">
         <v>758</v>
       </c>
-      <c r="B134" s="96" t="s">
+      <c r="B134" s="97" t="s">
         <v>2200</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>754</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E134" s="3"/>
     </row>
     <row r="135" ht="12.75" customHeight="1">
-      <c r="A135" s="96" t="s">
+      <c r="A135" s="97" t="s">
         <v>1542</v>
       </c>
-      <c r="B135" s="96" t="s">
-        <v>2307</v>
+      <c r="B135" s="97" t="s">
+        <v>2309</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>1099</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E135" s="3"/>
     </row>
     <row r="136" ht="12.75" customHeight="1">
-      <c r="A136" s="96" t="s">
+      <c r="A136" s="97" t="s">
         <v>1799</v>
       </c>
-      <c r="B136" s="96" t="s">
-        <v>2308</v>
+      <c r="B136" s="97" t="s">
+        <v>2310</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>1806</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E136" s="3"/>
     </row>
     <row r="137" ht="12.75" customHeight="1">
-      <c r="A137" s="96" t="s">
-        <v>2309</v>
-      </c>
-      <c r="B137" s="96" t="s">
-        <v>2310</v>
+      <c r="A137" s="97" t="s">
+        <v>2311</v>
+      </c>
+      <c r="B137" s="97" t="s">
+        <v>2312</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>1099</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E137" s="3"/>
     </row>
     <row r="138" ht="12.75" customHeight="1">
-      <c r="A138" s="96" t="s">
+      <c r="A138" s="97" t="s">
         <v>282</v>
       </c>
-      <c r="B138" s="96" t="s">
+      <c r="B138" s="97" t="s">
         <v>2201</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>1663</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E138" s="3"/>
     </row>
     <row r="139" ht="12.75" customHeight="1">
-      <c r="A139" s="96" t="s">
+      <c r="A139" s="97" t="s">
         <v>907</v>
       </c>
-      <c r="B139" s="96" t="s">
-        <v>2311</v>
+      <c r="B139" s="97" t="s">
+        <v>2313</v>
       </c>
       <c r="C139" s="3" t="s">
         <v>913</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E139" s="3"/>
     </row>
     <row r="140" ht="12.75" customHeight="1">
-      <c r="A140" s="96" t="s">
+      <c r="A140" s="97" t="s">
         <v>656</v>
       </c>
-      <c r="B140" s="96" t="s">
-        <v>2311</v>
+      <c r="B140" s="97" t="s">
+        <v>2313</v>
       </c>
       <c r="C140" s="3" t="s">
         <v>665</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E140" s="3"/>
     </row>
     <row r="141" ht="12.75" customHeight="1">
-      <c r="A141" s="96" t="s">
+      <c r="A141" s="97" t="s">
         <v>880</v>
       </c>
-      <c r="B141" s="96" t="s">
-        <v>2312</v>
+      <c r="B141" s="97" t="s">
+        <v>2314</v>
       </c>
       <c r="C141" s="3" t="s">
         <v>855</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E141" s="3"/>
     </row>
     <row r="142" ht="12.75" customHeight="1">
-      <c r="A142" s="96" t="s">
+      <c r="A142" s="97" t="s">
         <v>1905</v>
       </c>
-      <c r="B142" s="96" t="s">
-        <v>2313</v>
+      <c r="B142" s="97" t="s">
+        <v>2315</v>
       </c>
       <c r="C142" s="3" t="s">
         <v>1889</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E142" s="3"/>
     </row>
     <row r="143" ht="12.75" customHeight="1">
-      <c r="A143" s="96" t="s">
-        <v>2314</v>
-      </c>
-      <c r="B143" s="96" t="s">
-        <v>2313</v>
+      <c r="A143" s="97" t="s">
+        <v>2316</v>
+      </c>
+      <c r="B143" s="97" t="s">
+        <v>2315</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>1889</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E143" s="3"/>
     </row>
     <row r="144" ht="12.75" customHeight="1">
-      <c r="A144" s="96" t="s">
-        <v>2315</v>
-      </c>
-      <c r="B144" s="96" t="s">
-        <v>2316</v>
+      <c r="A144" s="97" t="s">
+        <v>2317</v>
+      </c>
+      <c r="B144" s="97" t="s">
+        <v>2318</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>1898</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E144" s="3"/>
     </row>
     <row r="145" ht="12.75" customHeight="1">
-      <c r="A145" s="96" t="s">
-        <v>2317</v>
-      </c>
-      <c r="B145" s="96" t="s">
-        <v>2316</v>
+      <c r="A145" s="97" t="s">
+        <v>2319</v>
+      </c>
+      <c r="B145" s="97" t="s">
+        <v>2318</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>1099</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E145" s="3"/>
     </row>
     <row r="146" ht="12.75" customHeight="1">
-      <c r="A146" s="96" t="s">
+      <c r="A146" s="97" t="s">
         <v>1888</v>
       </c>
-      <c r="B146" s="96" t="s">
-        <v>2318</v>
+      <c r="B146" s="97" t="s">
+        <v>2320</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>1889</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E146" s="3"/>
     </row>
     <row r="147" ht="12.75" customHeight="1">
-      <c r="A147" s="96" t="s">
+      <c r="A147" s="97" t="s">
         <v>1549</v>
       </c>
-      <c r="B147" s="96" t="s">
-        <v>2319</v>
+      <c r="B147" s="97" t="s">
+        <v>2321</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>1099</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E147" s="3"/>
     </row>
     <row r="148" ht="12.75" customHeight="1">
-      <c r="A148" s="96" t="s">
+      <c r="A148" s="97" t="s">
         <v>1255</v>
       </c>
-      <c r="B148" s="96" t="s">
-        <v>2320</v>
+      <c r="B148" s="97" t="s">
+        <v>2322</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>1329</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E148" s="3"/>
     </row>
     <row r="149" ht="12.75" customHeight="1">
-      <c r="A149" s="96" t="s">
+      <c r="A149" s="97" t="s">
         <v>941</v>
       </c>
-      <c r="B149" s="96" t="s">
-        <v>2321</v>
+      <c r="B149" s="97" t="s">
+        <v>2323</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>937</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E149" s="3"/>
     </row>
     <row r="150" ht="12.75" customHeight="1">
-      <c r="A150" s="96" t="s">
+      <c r="A150" s="97" t="s">
         <v>1044</v>
       </c>
-      <c r="B150" s="96" t="s">
-        <v>2322</v>
+      <c r="B150" s="97" t="s">
+        <v>2324</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>1022</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E150" s="3"/>
     </row>
     <row r="151" ht="12.75" customHeight="1">
-      <c r="A151" s="96" t="s">
+      <c r="A151" s="97" t="s">
         <v>1709</v>
       </c>
-      <c r="B151" s="96" t="s">
-        <v>2322</v>
+      <c r="B151" s="97" t="s">
+        <v>2324</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>1099</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E151" s="3"/>
     </row>
     <row r="152" ht="12.75" customHeight="1">
-      <c r="A152" s="96" t="s">
+      <c r="A152" s="97" t="s">
         <v>969</v>
       </c>
-      <c r="B152" s="96" t="s">
-        <v>2323</v>
+      <c r="B152" s="97" t="s">
+        <v>2325</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>981</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E152" s="3"/>
     </row>
     <row r="153" ht="12.75" customHeight="1">
-      <c r="A153" s="96" t="s">
+      <c r="A153" s="97" t="s">
         <v>1453</v>
       </c>
-      <c r="B153" s="96" t="s">
+      <c r="B153" s="97" t="s">
         <v>1455</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>1457</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E153" s="3"/>
     </row>
     <row r="154" ht="12.75" customHeight="1">
-      <c r="A154" s="96" t="s">
+      <c r="A154" s="97" t="s">
         <v>1088</v>
       </c>
-      <c r="B154" s="96" t="s">
+      <c r="B154" s="97" t="s">
         <v>1455</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>1069</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E154" s="3"/>
     </row>
     <row r="155" ht="12.75" customHeight="1">
-      <c r="A155" s="96" t="s">
-        <v>2324</v>
-      </c>
-      <c r="B155" s="96" t="s">
-        <v>2325</v>
+      <c r="A155" s="97" t="s">
+        <v>2326</v>
+      </c>
+      <c r="B155" s="97" t="s">
+        <v>2327</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>1193</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E155" s="3"/>
     </row>
     <row r="156" ht="12.75" customHeight="1">
-      <c r="A156" s="96" t="s">
+      <c r="A156" s="97" t="s">
         <v>1583</v>
       </c>
-      <c r="B156" s="96" t="s">
-        <v>2326</v>
+      <c r="B156" s="97" t="s">
+        <v>2328</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>1579</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="E156" s="3"/>
     </row>
@@ -34666,58 +34685,58 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="97" t="s">
-        <v>2327</v>
+      <c r="A1" s="98" t="s">
+        <v>2232</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="98" t="s">
-        <v>2328</v>
+      <c r="A2" s="99" t="s">
+        <v>2329</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>2329</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="98" t="s">
-        <v>2330</v>
+      <c r="A4" s="99" t="s">
+        <v>2331</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>2331</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>2332</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>2333</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="98" t="s">
-        <v>2334</v>
+      <c r="A8" s="99" t="s">
+        <v>2335</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>2335</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="18" t="s">
-        <v>2336</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>2337</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1"/>

</xml_diff>